<commit_message>
Grafico 2 Análise Censitária
</commit_message>
<xml_diff>
--- a/dados/umses_graduacao_2018_vtidy.xlsx
+++ b/dados/umses_graduacao_2018_vtidy.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11104"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jpalbino/Downloads/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E810EC-DBB5-B34C-A821-C084236E7F18}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25720" windowHeight="14940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="525" windowWidth="20730" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="dados" sheetId="1" r:id="rId1"/>
     <sheet name="dicionário de dados" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -586,7 +581,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1085,8 +1080,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Texto Explicativo" xfId="1" builtinId="53"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1144,7 +1139,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1196,7 +1191,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1390,23 +1385,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M56" sqref="M56"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1540,7 +1535,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
@@ -1668,7 +1663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -1796,7 +1791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1924,7 +1919,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2052,7 +2047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -2180,7 +2175,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -2308,7 +2303,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -2436,7 +2431,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -2564,7 +2559,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -2692,7 +2687,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2820,7 +2815,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2948,7 +2943,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -3076,7 +3071,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
@@ -3204,7 +3199,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -3332,7 +3327,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
       </c>
@@ -3460,7 +3455,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
@@ -3588,7 +3583,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2</v>
       </c>
@@ -3713,7 +3708,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -3838,7 +3833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2</v>
       </c>
@@ -3963,7 +3958,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>
@@ -4088,7 +4083,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2</v>
       </c>
@@ -4213,7 +4208,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2</v>
       </c>
@@ -4341,7 +4336,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2</v>
       </c>
@@ -4466,7 +4461,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
@@ -4591,7 +4586,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2</v>
       </c>
@@ -4716,7 +4711,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2</v>
       </c>
@@ -4841,7 +4836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3</v>
       </c>
@@ -4966,7 +4961,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2</v>
       </c>
@@ -5091,7 +5086,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>3</v>
       </c>
@@ -5219,7 +5214,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2</v>
       </c>
@@ -5344,7 +5339,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>3</v>
       </c>
@@ -5469,7 +5464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>3</v>
       </c>
@@ -5594,7 +5589,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2</v>
       </c>
@@ -5719,7 +5714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>3</v>
       </c>
@@ -5847,7 +5842,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2</v>
       </c>
@@ -5978,7 +5973,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>3</v>
       </c>
@@ -6103,7 +6098,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>3</v>
       </c>
@@ -6228,7 +6223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>3</v>
       </c>
@@ -6353,7 +6348,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2</v>
       </c>
@@ -6481,7 +6476,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2</v>
       </c>
@@ -6606,7 +6601,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2</v>
       </c>
@@ -6731,7 +6726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>3</v>
       </c>
@@ -6856,7 +6851,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>3</v>
       </c>
@@ -6981,7 +6976,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>3</v>
       </c>
@@ -7106,7 +7101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2</v>
       </c>
@@ -7231,7 +7226,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>3</v>
       </c>
@@ -7356,7 +7351,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2</v>
       </c>
@@ -7484,7 +7479,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2</v>
       </c>
@@ -7609,7 +7604,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2</v>
       </c>
@@ -7734,7 +7729,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2</v>
       </c>
@@ -7859,7 +7854,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2</v>
       </c>
@@ -7984,7 +7979,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2</v>
       </c>
@@ -8109,7 +8104,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2</v>
       </c>
@@ -8234,7 +8229,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>3</v>
       </c>
@@ -8362,7 +8357,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>3</v>
       </c>
@@ -8487,7 +8482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2</v>
       </c>
@@ -8612,7 +8607,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2</v>
       </c>
@@ -8737,7 +8732,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2</v>
       </c>
@@ -8865,7 +8860,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2</v>
       </c>
@@ -8990,7 +8985,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>3</v>
       </c>
@@ -9115,7 +9110,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>3</v>
       </c>
@@ -9247,24 +9242,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F117929-C34C-4710-88F8-3C03F7C91A17}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.5" customWidth="1"/>
-    <col min="2" max="2" width="21.5" customWidth="1"/>
-    <col min="3" max="3" width="89.5" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
-    <col min="5" max="5" width="31.1640625" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="89.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:5" ht="23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>54</v>
       </c>
@@ -9275,7 +9270,7 @@
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="66" t="s">
@@ -9284,7 +9279,7 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>55</v>
       </c>
@@ -9301,7 +9296,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>60</v>
       </c>
@@ -9310,7 +9305,7 @@
       <c r="D5" s="10"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="13" t="s">
         <v>0</v>
@@ -9325,7 +9320,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="13" t="s">
         <v>1</v>
@@ -9340,7 +9335,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
       <c r="B8" s="13" t="s">
         <v>67</v>
@@ -9355,7 +9350,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="136" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="13" t="s">
         <v>2</v>
@@ -9370,7 +9365,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
       <c r="B10" s="13" t="s">
         <v>3</v>
@@ -9385,7 +9380,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
       <c r="B11" s="13" t="s">
         <v>4</v>
@@ -9400,7 +9395,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="205" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="186" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="13" t="s">
         <v>5</v>
@@ -9415,7 +9410,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>80</v>
       </c>
@@ -9424,7 +9419,7 @@
       <c r="D13" s="20"/>
       <c r="E13" s="19"/>
     </row>
-    <row r="14" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
       <c r="B14" s="22" t="s">
         <v>81</v>
@@ -9437,7 +9432,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="21"/>
       <c r="B15" s="22" t="s">
         <v>83</v>
@@ -9450,7 +9445,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="21"/>
       <c r="B16" s="22" t="s">
         <v>84</v>
@@ -9463,7 +9458,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="21"/>
       <c r="B17" s="22" t="s">
         <v>85</v>
@@ -9476,7 +9471,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="21"/>
       <c r="B18" s="22" t="s">
         <v>86</v>
@@ -9489,7 +9484,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="21"/>
       <c r="B19" s="22" t="s">
         <v>87</v>
@@ -9502,7 +9497,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="21"/>
       <c r="B20" s="22" t="s">
         <v>88</v>
@@ -9515,7 +9510,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="21"/>
       <c r="B21" s="22" t="s">
         <v>89</v>
@@ -9528,7 +9523,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="21"/>
       <c r="B22" s="22" t="s">
         <v>90</v>
@@ -9541,7 +9536,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="21"/>
       <c r="B23" s="25" t="s">
         <v>15</v>
@@ -9552,7 +9547,7 @@
       <c r="D23" s="26"/>
       <c r="E23" s="26"/>
     </row>
-    <row r="24" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
         <v>92</v>
       </c>
@@ -9561,7 +9556,7 @@
       <c r="D24" s="29"/>
       <c r="E24" s="28"/>
     </row>
-    <row r="25" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="30"/>
       <c r="B25" s="31" t="s">
         <v>16</v>
@@ -9576,7 +9571,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="30"/>
       <c r="B26" s="31" t="s">
         <v>17</v>
@@ -9591,7 +9586,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="30"/>
       <c r="B27" s="31" t="s">
         <v>18</v>
@@ -9606,7 +9601,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="30"/>
       <c r="B28" s="31" t="s">
         <v>19</v>
@@ -9621,7 +9616,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="30"/>
       <c r="B29" s="31" t="s">
         <v>20</v>
@@ -9636,7 +9631,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="30"/>
       <c r="B30" s="31" t="s">
         <v>21</v>
@@ -9651,7 +9646,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="30"/>
       <c r="B31" s="31" t="s">
         <v>22</v>
@@ -9666,7 +9661,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="30"/>
       <c r="B32" s="31" t="s">
         <v>23</v>
@@ -9681,7 +9676,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="30"/>
       <c r="B33" s="31" t="s">
         <v>24</v>
@@ -9696,7 +9691,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="30"/>
       <c r="B34" s="31" t="s">
         <v>25</v>
@@ -9711,7 +9706,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="34"/>
       <c r="B35" s="31" t="s">
         <v>26</v>
@@ -9726,7 +9721,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="38" t="s">
         <v>106</v>
       </c>
@@ -9735,7 +9730,7 @@
       <c r="D36" s="40"/>
       <c r="E36" s="28"/>
     </row>
-    <row r="37" spans="1:5" ht="153" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A37" s="41"/>
       <c r="B37" s="42" t="s">
         <v>27</v>
@@ -9750,7 +9745,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" s="45"/>
       <c r="B38" s="42" t="s">
         <v>28</v>
@@ -9765,7 +9760,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="45"/>
       <c r="B39" s="42" t="s">
         <v>29</v>
@@ -9780,7 +9775,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="45"/>
       <c r="B40" s="42" t="s">
         <v>30</v>
@@ -9795,7 +9790,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A41" s="46" t="s">
         <v>116</v>
       </c>
@@ -9804,7 +9799,7 @@
       <c r="D41" s="48"/>
       <c r="E41" s="48"/>
     </row>
-    <row r="42" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="49"/>
       <c r="B42" s="50" t="s">
         <v>31</v>
@@ -9819,7 +9814,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="49"/>
       <c r="B43" s="50" t="s">
         <v>32</v>
@@ -9834,7 +9829,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="49"/>
       <c r="B44" s="50" t="s">
         <v>33</v>
@@ -9849,7 +9844,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="49"/>
       <c r="B45" s="50" t="s">
         <v>34</v>
@@ -9864,7 +9859,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="49"/>
       <c r="B46" s="50" t="s">
         <v>35</v>
@@ -9879,7 +9874,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A47" s="53"/>
       <c r="B47" s="54" t="s">
         <v>36</v>
@@ -9894,7 +9889,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="38" t="s">
         <v>123</v>
       </c>
@@ -9903,7 +9898,7 @@
       <c r="D48" s="28"/>
       <c r="E48" s="28"/>
     </row>
-    <row r="49" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" s="59"/>
       <c r="B49" s="60" t="s">
         <v>37</v>
@@ -9918,7 +9913,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A50" s="59"/>
       <c r="B50" s="60" t="s">
         <v>38</v>
@@ -9933,7 +9928,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" s="59"/>
       <c r="B51" s="60" t="s">
         <v>39</v>
@@ -9948,7 +9943,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A52" s="59"/>
       <c r="B52" s="60" t="s">
         <v>40</v>
@@ -9963,7 +9958,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A53" s="59"/>
       <c r="B53" s="60" t="s">
         <v>41</v>
@@ -9978,7 +9973,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="86" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="62"/>
       <c r="B54" s="63" t="s">
         <v>42</v>
@@ -9997,4 +9992,18 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>